<commit_message>
Modified formatting of spreadsheet (just aesthetics stuff)
</commit_message>
<xml_diff>
--- a/src/main/resources/Invoice_Template.xlsx
+++ b/src/main/resources/Invoice_Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidkim/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidkim/IdeaProjects/webportal/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16220"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17480"/>
   </bookViews>
   <sheets>
     <sheet name="Finance Charge" sheetId="1" r:id="rId1"/>
@@ -457,61 +457,39 @@
     <xf numFmtId="44" fontId="9" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -531,26 +509,48 @@
     <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -658,7 +658,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -689,7 +689,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40dd-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -718,7 +718,7 @@
         <xdr:cNvPr id="1029" name="Text Box 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000005040000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -744,7 +744,7 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{91240B29-F687-4f45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
               </a:solidFill>
@@ -1063,7 +1063,7 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="A17" sqref="A17:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1080,210 +1080,210 @@
   <sheetData>
     <row r="1" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5"/>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
       <c r="E1" s="25"/>
-      <c r="F1" s="65" t="s">
+      <c r="F1" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
     </row>
     <row r="2" spans="1:8" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="69"/>
-      <c r="B2" s="70"/>
+      <c r="A2" s="61"/>
+      <c r="B2" s="62"/>
       <c r="C2" s="23"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
     </row>
     <row r="3" spans="1:8" s="4" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="68"/>
+      <c r="B3" s="60"/>
       <c r="C3" s="22"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="63"/>
-      <c r="B4" s="63"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="60"/>
+      <c r="B5" s="55"/>
       <c r="C5" s="21"/>
       <c r="D5" s="32"/>
       <c r="E5" s="32"/>
       <c r="F5" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
     </row>
     <row r="6" spans="1:8" s="4" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="60"/>
+      <c r="B6" s="55"/>
       <c r="C6" s="21"/>
       <c r="D6" s="32"/>
       <c r="E6" s="32"/>
       <c r="F6" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
     </row>
     <row r="7" spans="1:8" s="4" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="60" t="s">
+      <c r="A7" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="60"/>
+      <c r="B7" s="55"/>
       <c r="C7" s="21"/>
-      <c r="D7" s="61" t="s">
+      <c r="D7" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
     </row>
     <row r="8" spans="1:8" s="4" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="60" t="s">
+      <c r="A8" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="60"/>
+      <c r="B8" s="55"/>
       <c r="C8" s="21"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="62"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:8" s="4" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="62"/>
-      <c r="B9" s="62"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="62"/>
+      <c r="A9" s="65"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
     </row>
     <row r="10" spans="1:8" s="4" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="63"/>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
       <c r="E10" s="24"/>
       <c r="F10" s="19"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
     </row>
     <row r="11" spans="1:8" s="4" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="8"/>
-      <c r="B11" s="63"/>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
       <c r="E11" s="24"/>
       <c r="F11" s="9"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
     </row>
     <row r="12" spans="1:8" s="4" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9"/>
-      <c r="B12" s="63"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="63"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="47"/>
+      <c r="D12" s="47"/>
       <c r="E12" s="24"/>
       <c r="F12" s="9"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
     </row>
     <row r="13" spans="1:8" s="4" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="63"/>
-      <c r="D13" s="63"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
       <c r="E13" s="24"/>
       <c r="F13" s="9"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
     </row>
     <row r="14" spans="1:8" s="4" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9"/>
-      <c r="B14" s="63"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="47"/>
+      <c r="D14" s="47"/>
       <c r="E14" s="24"/>
       <c r="F14" s="9"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
     </row>
     <row r="15" spans="1:8" s="4" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="56"/>
-      <c r="B15" s="56"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="56"/>
-      <c r="H15" s="56"/>
+      <c r="A15" s="52"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="52"/>
     </row>
     <row r="16" spans="1:8" s="4" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="56"/>
-      <c r="B16" s="56"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="56"/>
+      <c r="A16" s="52"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
     </row>
     <row r="17" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="57"/>
-      <c r="B17" s="58"/>
-      <c r="C17" s="58"/>
-      <c r="D17" s="58"/>
-      <c r="E17" s="58"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="59"/>
+      <c r="A17" s="72"/>
+      <c r="B17" s="73"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="73"/>
+      <c r="H17" s="74"/>
     </row>
     <row r="18" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="78"/>
-      <c r="B18" s="78"/>
-      <c r="C18" s="78"/>
-      <c r="D18" s="78"/>
-      <c r="E18" s="78"/>
-      <c r="F18" s="78"/>
-      <c r="G18" s="76"/>
-      <c r="H18" s="76"/>
+      <c r="A18" s="54"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="51"/>
+      <c r="H18" s="51"/>
     </row>
     <row r="19" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="54" t="s">
+      <c r="A19" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="55"/>
-      <c r="C19" s="55"/>
+      <c r="B19" s="71"/>
+      <c r="C19" s="71"/>
       <c r="D19" s="34" t="s">
         <v>7</v>
       </c>
@@ -1293,210 +1293,210 @@
       <c r="F19" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="77" t="s">
+      <c r="G19" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="H19" s="77"/>
+      <c r="H19" s="53"/>
     </row>
     <row r="20" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="46"/>
-      <c r="B20" s="47"/>
-      <c r="C20" s="47"/>
+      <c r="A20" s="68"/>
+      <c r="B20" s="69"/>
+      <c r="C20" s="69"/>
       <c r="D20" s="26"/>
       <c r="E20" s="40"/>
       <c r="F20" s="36"/>
-      <c r="G20" s="74"/>
-      <c r="H20" s="74"/>
+      <c r="G20" s="49"/>
+      <c r="H20" s="49"/>
     </row>
     <row r="21" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="44"/>
-      <c r="B21" s="45"/>
-      <c r="C21" s="45"/>
+      <c r="A21" s="66"/>
+      <c r="B21" s="67"/>
+      <c r="C21" s="67"/>
       <c r="D21" s="27"/>
       <c r="E21" s="41"/>
       <c r="F21" s="37"/>
-      <c r="G21" s="75"/>
-      <c r="H21" s="75"/>
+      <c r="G21" s="50"/>
+      <c r="H21" s="50"/>
     </row>
     <row r="22" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="46"/>
-      <c r="B22" s="47"/>
-      <c r="C22" s="47"/>
+      <c r="A22" s="68"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="69"/>
       <c r="D22" s="26"/>
       <c r="E22" s="40"/>
       <c r="F22" s="36"/>
-      <c r="G22" s="74"/>
-      <c r="H22" s="74"/>
+      <c r="G22" s="49"/>
+      <c r="H22" s="49"/>
     </row>
     <row r="23" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="44"/>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
+      <c r="A23" s="66"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="67"/>
       <c r="D23" s="29"/>
       <c r="E23" s="43"/>
       <c r="F23" s="39"/>
-      <c r="G23" s="49"/>
-      <c r="H23" s="49"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="48"/>
     </row>
     <row r="24" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="46"/>
-      <c r="B24" s="47"/>
-      <c r="C24" s="47"/>
+      <c r="A24" s="68"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="69"/>
       <c r="D24" s="28"/>
       <c r="E24" s="42"/>
       <c r="F24" s="38"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
+      <c r="G24" s="77"/>
+      <c r="H24" s="77"/>
     </row>
     <row r="25" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="44"/>
-      <c r="B25" s="45"/>
-      <c r="C25" s="45"/>
+      <c r="A25" s="66"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="67"/>
       <c r="D25" s="29"/>
       <c r="E25" s="43"/>
       <c r="F25" s="39"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="49"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="48"/>
     </row>
     <row r="26" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="46"/>
-      <c r="B26" s="47"/>
-      <c r="C26" s="47"/>
+      <c r="A26" s="68"/>
+      <c r="B26" s="69"/>
+      <c r="C26" s="69"/>
       <c r="D26" s="28"/>
       <c r="E26" s="42"/>
       <c r="F26" s="38"/>
-      <c r="G26" s="48"/>
-      <c r="H26" s="48"/>
+      <c r="G26" s="77"/>
+      <c r="H26" s="77"/>
     </row>
     <row r="27" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="44"/>
-      <c r="B27" s="45"/>
-      <c r="C27" s="45"/>
+      <c r="A27" s="66"/>
+      <c r="B27" s="67"/>
+      <c r="C27" s="67"/>
       <c r="D27" s="29"/>
       <c r="E27" s="43"/>
       <c r="F27" s="39"/>
-      <c r="G27" s="49"/>
-      <c r="H27" s="49"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="48"/>
     </row>
     <row r="28" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="46"/>
-      <c r="B28" s="47"/>
-      <c r="C28" s="47"/>
+      <c r="A28" s="68"/>
+      <c r="B28" s="69"/>
+      <c r="C28" s="69"/>
       <c r="D28" s="28"/>
       <c r="E28" s="42"/>
       <c r="F28" s="38"/>
-      <c r="G28" s="48"/>
-      <c r="H28" s="48"/>
+      <c r="G28" s="77"/>
+      <c r="H28" s="77"/>
     </row>
     <row r="29" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="44"/>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
+      <c r="A29" s="66"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="67"/>
       <c r="D29" s="29"/>
       <c r="E29" s="43"/>
       <c r="F29" s="39"/>
-      <c r="G29" s="49"/>
-      <c r="H29" s="49"/>
+      <c r="G29" s="48"/>
+      <c r="H29" s="48"/>
     </row>
     <row r="30" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="46"/>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
+      <c r="A30" s="68"/>
+      <c r="B30" s="69"/>
+      <c r="C30" s="69"/>
       <c r="D30" s="28"/>
       <c r="E30" s="42"/>
       <c r="F30" s="38"/>
-      <c r="G30" s="48"/>
-      <c r="H30" s="48"/>
+      <c r="G30" s="77"/>
+      <c r="H30" s="77"/>
     </row>
     <row r="31" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="44"/>
-      <c r="B31" s="45"/>
-      <c r="C31" s="45"/>
+      <c r="A31" s="66"/>
+      <c r="B31" s="67"/>
+      <c r="C31" s="67"/>
       <c r="D31" s="29"/>
       <c r="E31" s="43"/>
       <c r="F31" s="39"/>
-      <c r="G31" s="49"/>
-      <c r="H31" s="49"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48"/>
     </row>
     <row r="32" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="46"/>
-      <c r="B32" s="47"/>
-      <c r="C32" s="47"/>
+      <c r="A32" s="68"/>
+      <c r="B32" s="69"/>
+      <c r="C32" s="69"/>
       <c r="D32" s="28"/>
       <c r="E32" s="42"/>
       <c r="F32" s="38"/>
-      <c r="G32" s="48"/>
-      <c r="H32" s="48"/>
+      <c r="G32" s="77"/>
+      <c r="H32" s="77"/>
     </row>
     <row r="33" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="44"/>
-      <c r="B33" s="45"/>
-      <c r="C33" s="45"/>
+      <c r="A33" s="66"/>
+      <c r="B33" s="67"/>
+      <c r="C33" s="67"/>
       <c r="D33" s="29"/>
       <c r="E33" s="43"/>
       <c r="F33" s="39"/>
-      <c r="G33" s="49"/>
-      <c r="H33" s="49"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="48"/>
     </row>
     <row r="34" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="46"/>
-      <c r="B34" s="47"/>
-      <c r="C34" s="47"/>
+      <c r="A34" s="68"/>
+      <c r="B34" s="69"/>
+      <c r="C34" s="69"/>
       <c r="D34" s="28"/>
       <c r="E34" s="42"/>
       <c r="F34" s="38"/>
-      <c r="G34" s="48"/>
-      <c r="H34" s="48"/>
+      <c r="G34" s="77"/>
+      <c r="H34" s="77"/>
     </row>
     <row r="35" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="44"/>
-      <c r="B35" s="45"/>
-      <c r="C35" s="45"/>
+      <c r="A35" s="66"/>
+      <c r="B35" s="67"/>
+      <c r="C35" s="67"/>
       <c r="D35" s="29"/>
       <c r="E35" s="43"/>
       <c r="F35" s="39"/>
-      <c r="G35" s="49"/>
-      <c r="H35" s="49"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="48"/>
     </row>
     <row r="36" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="46"/>
-      <c r="B36" s="47"/>
-      <c r="C36" s="47"/>
+      <c r="A36" s="68"/>
+      <c r="B36" s="69"/>
+      <c r="C36" s="69"/>
       <c r="D36" s="28"/>
       <c r="E36" s="42"/>
       <c r="F36" s="38"/>
-      <c r="G36" s="52"/>
-      <c r="H36" s="52"/>
+      <c r="G36" s="78"/>
+      <c r="H36" s="78"/>
     </row>
     <row r="37" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="44"/>
-      <c r="B37" s="45"/>
-      <c r="C37" s="45"/>
+      <c r="A37" s="66"/>
+      <c r="B37" s="67"/>
+      <c r="C37" s="67"/>
       <c r="D37" s="29"/>
       <c r="E37" s="43"/>
       <c r="F37" s="39"/>
-      <c r="G37" s="49"/>
-      <c r="H37" s="49"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="48"/>
     </row>
     <row r="38" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="46"/>
-      <c r="B38" s="47"/>
-      <c r="C38" s="47"/>
+      <c r="A38" s="68"/>
+      <c r="B38" s="69"/>
+      <c r="C38" s="69"/>
       <c r="D38" s="28"/>
       <c r="E38" s="42"/>
       <c r="F38" s="38"/>
-      <c r="G38" s="52"/>
-      <c r="H38" s="52"/>
+      <c r="G38" s="78"/>
+      <c r="H38" s="78"/>
     </row>
     <row r="39" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="44"/>
-      <c r="B39" s="45"/>
-      <c r="C39" s="45"/>
+      <c r="A39" s="66"/>
+      <c r="B39" s="67"/>
+      <c r="C39" s="67"/>
       <c r="D39" s="29"/>
       <c r="E39" s="43"/>
       <c r="F39" s="39"/>
-      <c r="G39" s="49"/>
-      <c r="H39" s="49"/>
+      <c r="G39" s="48"/>
+      <c r="H39" s="48"/>
     </row>
     <row r="40" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="30"/>
@@ -1507,11 +1507,11 @@
       <c r="F40" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G40" s="50" t="str">
+      <c r="G40" s="75" t="str">
         <f>IF(SUM(G20:G39)&gt;0,SUM(G20:G39),"")</f>
         <v/>
       </c>
-      <c r="H40" s="51"/>
+      <c r="H40" s="76"/>
     </row>
     <row r="41" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="11"/>
@@ -1537,26 +1537,26 @@
       </c>
     </row>
     <row r="43" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="72" t="s">
+      <c r="A43" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="B43" s="73"/>
-      <c r="C43" s="73"/>
-      <c r="D43" s="73"/>
-      <c r="E43" s="73"/>
-      <c r="F43" s="73"/>
-      <c r="G43" s="73"/>
-      <c r="H43" s="73"/>
+      <c r="B43" s="45"/>
+      <c r="C43" s="45"/>
+      <c r="D43" s="45"/>
+      <c r="E43" s="45"/>
+      <c r="F43" s="45"/>
+      <c r="G43" s="45"/>
+      <c r="H43" s="45"/>
     </row>
     <row r="44" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="73"/>
-      <c r="B44" s="73"/>
-      <c r="C44" s="73"/>
-      <c r="D44" s="73"/>
-      <c r="E44" s="73"/>
-      <c r="F44" s="73"/>
-      <c r="G44" s="73"/>
-      <c r="H44" s="73"/>
+      <c r="A44" s="45"/>
+      <c r="B44" s="45"/>
+      <c r="C44" s="45"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="45"/>
+      <c r="G44" s="45"/>
+      <c r="H44" s="45"/>
     </row>
     <row r="45" spans="1:8" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="9"/>
@@ -1581,6 +1581,66 @@
     </row>
   </sheetData>
   <mergeCells count="76">
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="D2:H2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
     <mergeCell ref="A43:H44"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="G12:H12"/>
@@ -1597,70 +1657,10 @@
     <mergeCell ref="G19:H19"/>
     <mergeCell ref="G20:H20"/>
     <mergeCell ref="A18:F18"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="A9:H9"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A39:C39"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.75" right="0.75" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
+  <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>